<commit_message>
22/12/2022 - Tabla MicroPy vs C
</commit_message>
<xml_diff>
--- a/Words y Excel/Comparativas.xlsx
+++ b/Words y Excel/Comparativas.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Placas" sheetId="1" r:id="rId1"/>
-    <sheet name="Max30100_21" sheetId="2" r:id="rId2"/>
+    <sheet name="ESP32_Lenguaje" sheetId="3" r:id="rId2"/>
+    <sheet name="Max30100_21" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t>Bitalino</t>
   </si>
@@ -289,6 +290,64 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Lenguaje</t>
+  </si>
+  <si>
+    <t>MicroPython</t>
+  </si>
+  <si>
+    <t>C
+(En Arduino-IDE)</t>
+  </si>
+  <si>
+    <t>Importar 
+Bilbiotecas</t>
+  </si>
+  <si>
+    <t>Velocidad</t>
+  </si>
+  <si>
+    <t>Más Lento</t>
+  </si>
+  <si>
+    <t>Más Rápido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliotecas
+Tiempo-Real </t>
+  </si>
+  <si>
+    <t>Sí, tiene</t>
+  </si>
+  <si>
+    <t>Sí, puede</t>
+  </si>
+  <si>
+    <t>Compilación</t>
+  </si>
+  <si>
+    <t>En cada
+modificación 
+del programa</t>
+  </si>
+  <si>
+    <t>Mediante un 
+sistema de
+archivos</t>
+  </si>
+  <si>
+    <t>Portabilidad
+(a otros disp.)</t>
+  </si>
+  <si>
+    <t>Completa</t>
+  </si>
+  <si>
+    <t>En
+circustancias
+específicas</t>
   </si>
 </sst>
 </file>
@@ -457,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -480,22 +539,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,6 +566,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -521,9 +586,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1073,6 +1135,260 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197954</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3073" name="AutoShape 1" descr="Funciones en Lenguaje C - Declaración, sintaxis y ejemplos"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3048000" y="1714500"/>
+          <a:ext cx="3105150" cy="1476375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>477841</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1047186</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>712305</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="MicroPython - Wikipedia, la enciclopedia libre"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2001841" y="704022"/>
+          <a:ext cx="569345" cy="579783"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>259407</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>182980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1350067</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>633832</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Grupo 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2172690" y="1847784"/>
+          <a:ext cx="1090660" cy="450852"/>
+          <a:chOff x="3774098" y="1822938"/>
+          <a:chExt cx="2910380" cy="1203080"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Imagen 2" descr="Funciones en Lenguaje C - Declaración, sintaxis y ejemplos"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+            <a:extLst>
+              <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a14:imgLayer r:embed="rId3">
+                    <a14:imgEffect>
+                      <a14:backgroundRemoval t="2105" b="100000" l="10000" r="90000">
+                        <a14:foregroundMark x1="47500" y1="30263" x2="47500" y2="30263"/>
+                        <a14:foregroundMark x1="54625" y1="31053" x2="56875" y2="38947"/>
+                        <a14:foregroundMark x1="53875" y1="32368" x2="45750" y2="29211"/>
+                        <a14:foregroundMark x1="43875" y1="35263" x2="40875" y2="56842"/>
+                        <a14:foregroundMark x1="41625" y1="62895" x2="47500" y2="76316"/>
+                      </a14:backgroundRemoval>
+                    </a14:imgEffect>
+                  </a14:imgLayer>
+                </a14:imgProps>
+              </a:ext>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="27750" r="28875"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="3774098" y="1876424"/>
+            <a:ext cx="976165" cy="1068999"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Imagen 4" descr="Nuevo IDE de Arduino versión 2.0 disponible públicamente"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+            <a:extLst>
+              <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a14:imgLayer r:embed="rId5">
+                    <a14:imgEffect>
+                      <a14:backgroundRemoval t="9398" b="89850" l="1500" r="92000">
+                        <a14:foregroundMark x1="14000" y1="42857" x2="17000" y2="43233"/>
+                        <a14:foregroundMark x1="34750" y1="43233" x2="38250" y2="43233"/>
+                        <a14:foregroundMark x1="9500" y1="66917" x2="9500" y2="66917"/>
+                        <a14:foregroundMark x1="15250" y1="66541" x2="15250" y2="66541"/>
+                        <a14:foregroundMark x1="19000" y1="69925" x2="19000" y2="69925"/>
+                        <a14:foregroundMark x1="28500" y1="68421" x2="28500" y2="68421"/>
+                        <a14:foregroundMark x1="33500" y1="62782" x2="33500" y2="62782"/>
+                        <a14:foregroundMark x1="37000" y1="63910" x2="37000" y2="63910"/>
+                        <a14:foregroundMark x1="44000" y1="62406" x2="44000" y2="62406"/>
+                        <a14:foregroundMark x1="72750" y1="45489" x2="72750" y2="45489"/>
+                        <a14:foregroundMark x1="69750" y1="30827" x2="69750" y2="30827"/>
+                        <a14:foregroundMark x1="69500" y1="24436" x2="69500" y2="24436"/>
+                        <a14:foregroundMark x1="74000" y1="24812" x2="74000" y2="24812"/>
+                        <a14:foregroundMark x1="84000" y1="24436" x2="84000" y2="24436"/>
+                        <a14:foregroundMark x1="85000" y1="41729" x2="85000" y2="41729"/>
+                        <a14:foregroundMark x1="79000" y1="67669" x2="79000" y2="67669"/>
+                        <a14:foregroundMark x1="46500" y1="30075" x2="46500" y2="30075"/>
+                        <a14:foregroundMark x1="45250" y1="30451" x2="45250" y2="30451"/>
+                        <a14:foregroundMark x1="45000" y1="28947" x2="47000" y2="30075"/>
+                        <a14:foregroundMark x1="44750" y1="28947" x2="47000" y2="30827"/>
+                      </a14:backgroundRemoval>
+                    </a14:imgEffect>
+                  </a14:imgLayer>
+                </a14:imgProps>
+              </a:ext>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="4875335" y="1822938"/>
+            <a:ext cx="1809143" cy="1203080"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -1513,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1532,60 +1848,60 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="14" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="10"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="17"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="6" t="s">
         <v>43</v>
       </c>
@@ -1595,7 +1911,7 @@
       <c r="L5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -1634,7 +1950,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1670,7 +1986,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1776,60 +2092,60 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="14" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="10"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="17"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="6" t="s">
         <v>30</v>
       </c>
@@ -1839,7 +2155,7 @@
       <c r="L15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="11"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
@@ -1878,7 +2194,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1914,7 +2230,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
@@ -2021,12 +2337,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E3:L3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M3:M5"/>
     <mergeCell ref="B13:B15"/>
@@ -2043,6 +2353,12 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C3:D5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" display="https://www.pluxbiosignals.com/collections/teaching-kits/products/bitalino-revolution-board-kit-ble-bt"/>
@@ -2064,10 +2380,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
+    <col min="4" max="8" width="14.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E10"/>
+      <c r="I10"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,31 +2509,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="9" t="s">
         <v>73</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -2155,31 +2583,31 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="9" t="s">
         <v>77</v>
       </c>
       <c r="H10" s="6" t="s">

</xml_diff>